<commit_message>
Changed config file to orchestrator assets, sending email after order complete
</commit_message>
<xml_diff>
--- a/OrderProcess/Orders.xlsx
+++ b/OrderProcess/Orders.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6848AD67-21E0-48FE-8437-4BFF2EE28563}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115C8BFA-F11E-40FB-8631-06D042481DE2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Product</t>
   </si>
@@ -84,22 +84,26 @@
   </si>
   <si>
     <t>701 W Mithcel Cir, 238 D</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Order Number: 512464</t>
+  </si>
+  <si>
+    <t>Erro</t>
+  </si>
+  <si>
+    <t>Product Ipoh Coff not Found</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -127,12 +131,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,19 +415,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,72 +439,117 @@
       <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
       </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="2">
         <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>